<commit_message>
Updated BOM file for PermaProto cell version
There is no Instructable for this version, but the BOM spreadsheet is updated for alternate parts
</commit_message>
<xml_diff>
--- a/docs/IV_Swinger2/Perma_Proto_construction/IV_Swinger2_Cell_Version_BOM.xlsx
+++ b/docs/IV_Swinger2/Perma_Proto_construction/IV_Swinger2_Cell_Version_BOM.xlsx
@@ -1,19 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csatt/GitHub/IV_Swinger/docs/IV_Swinger2/Perma_Proto_construction/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6062874-33FE-934F-9921-358C4265DB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="1400" windowWidth="25880" windowHeight="18900" tabRatio="500"/>
+    <workbookView xWindow="7040" yWindow="1400" windowWidth="31400" windowHeight="25060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$1:$F$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$2:$F$40</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
   <si>
     <t>Description</t>
   </si>
@@ -262,17 +275,20 @@
   </si>
   <si>
     <t>need two for cell version</t>
+  </si>
+  <si>
+    <t>NOTE: The prices and other details below are out of date. The PermaProto based cell version IVS2 is deprecated. The PCB-based cell versions are somewhat supported, but in reality no one has built them, so they are effectively deprecated too.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -339,6 +355,7 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -362,6 +379,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -382,7 +407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -414,6 +439,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -677,7 +711,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -733,21 +767,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -782,6 +801,24 @@
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="260">
@@ -1048,6 +1085,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1372,17 +1417,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="55" style="10" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="10"/>
@@ -1394,476 +1439,464 @@
     <col min="8" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="88" customHeight="1">
+      <c r="A1" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="22" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-    </row>
-    <row r="3" spans="1:7" ht="25">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+    </row>
+    <row r="4" spans="1:7" ht="23">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B4" s="21">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C4" s="6">
         <v>2.67</v>
       </c>
-      <c r="D3" s="6">
-        <f t="shared" ref="D3:D10" si="0">B3*C3</f>
+      <c r="D4" s="6">
+        <f t="shared" ref="D4:D11" si="0">B4*C4</f>
         <v>5.34</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G4" s="30" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="69">
-      <c r="A4" s="27" t="s">
+    <row r="5" spans="1:7" ht="75">
+      <c r="A5" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C5" s="23">
         <v>7.99</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D5" s="23">
         <f t="shared" si="0"/>
         <v>7.99</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F5" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G5" s="30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="25">
-      <c r="A5" s="27" t="s">
+    <row r="6" spans="1:7" ht="25">
+      <c r="A6" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B6" s="21">
         <v>2</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C6" s="23">
         <v>3.49</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D6" s="23">
         <f t="shared" si="0"/>
         <v>6.98</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F6" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G6" s="30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
-      <c r="A6" s="30" t="s">
+    <row r="7" spans="1:7" ht="34">
+      <c r="A7" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B7" s="26">
         <v>0</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C7" s="27">
         <f>6.99/5</f>
         <v>1.3980000000000001</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D7" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E7" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F7" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G7" s="30" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45">
-      <c r="A7" s="33" t="s">
+    <row r="8" spans="1:7" ht="51">
+      <c r="A8" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B8" s="26">
         <v>0</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C8" s="27">
         <v>0.78</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D8" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E8" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F8" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G8" s="30" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:7" ht="68">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C9" s="6">
         <f>(7.99/25)*3</f>
         <v>0.95879999999999999</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="6">
         <f t="shared" si="0"/>
         <v>0.95879999999999999</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G9" s="31" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:7" ht="34">
+      <c r="A10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B10" s="21">
         <v>1</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C10" s="6">
         <f>8.89/20</f>
         <v>0.44450000000000001</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D10" s="6">
         <f t="shared" si="0"/>
         <v>0.44450000000000001</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G10" s="31" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:7" ht="34">
+      <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B11" s="5">
         <v>2</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C11" s="6">
         <v>0.18</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D11" s="6">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-    </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+    </row>
+    <row r="14" spans="1:7" ht="17">
+      <c r="A14" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6">
-        <v>2.98</v>
-      </c>
-      <c r="D13" s="6">
-        <f t="shared" ref="D13:D24" si="1">B13*C13</f>
-        <v>2.98</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
       </c>
       <c r="C14" s="6">
+        <v>2.98</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" ref="D14:D25" si="1">B14*C14</f>
+        <v>2.98</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17">
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6">
         <v>2.58</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D15" s="6">
         <f t="shared" si="1"/>
         <v>2.58</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:7" ht="17">
+      <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B16" s="5">
         <v>1</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C16" s="6">
         <v>2.0499999999999998</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D16" s="6">
         <f t="shared" si="1"/>
         <v>2.0499999999999998</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:7" ht="17">
+      <c r="A17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B17" s="5">
         <v>2</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C17" s="19">
         <v>0.18</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D17" s="6">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:7" ht="17">
+      <c r="A18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B18" s="5">
         <v>2</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C18" s="6">
         <f>7.46/60</f>
         <v>0.12433333333333334</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D18" s="6">
         <f t="shared" si="1"/>
         <v>0.24866666666666667</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="33" t="s">
+    <row r="19" spans="1:7" ht="17">
+      <c r="A19" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B19" s="26">
         <v>1</v>
       </c>
-      <c r="C18" s="37">
+      <c r="C19" s="32">
         <f>9.59/1280</f>
         <v>7.4921874999999997E-3</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D19" s="27">
         <f t="shared" si="1"/>
         <v>7.4921874999999997E-3</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="F19" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="35" t="s">
+      <c r="G19" s="30" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="33" t="s">
+    <row r="20" spans="1:7" ht="17">
+      <c r="A20" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="31">
+      <c r="B20" s="26">
         <v>1</v>
       </c>
-      <c r="C19" s="37">
-        <f t="shared" ref="C19:C23" si="2">9.59/1280</f>
+      <c r="C20" s="32">
+        <f t="shared" ref="C20:C24" si="2">9.59/1280</f>
         <v>7.4921874999999997E-3</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D20" s="27">
         <f t="shared" si="1"/>
         <v>7.4921874999999997E-3</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E20" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F20" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="35" t="s">
+      <c r="G20" s="30" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="4" t="s">
+    <row r="21" spans="1:7" ht="17">
+      <c r="A21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B21" s="5">
         <v>1</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C21" s="19">
         <f t="shared" si="2"/>
         <v>7.4921874999999997E-3</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D21" s="6">
         <f t="shared" si="1"/>
         <v>7.4921874999999997E-3</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="25">
-      <c r="A21" s="27" t="s">
+    <row r="22" spans="1:7" ht="25">
+      <c r="A22" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B22" s="21">
         <v>1</v>
       </c>
-      <c r="C21" s="38">
+      <c r="C22" s="33">
         <f t="shared" si="2"/>
         <v>7.4921874999999997E-3</v>
       </c>
-      <c r="D21" s="28">
-        <f t="shared" ref="D21" si="3">B21*C21</f>
+      <c r="D22" s="23">
+        <f t="shared" ref="D22" si="3">B22*C22</f>
         <v>7.4921874999999997E-3</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E22" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F22" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G22" s="30" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:7" ht="17">
+      <c r="A23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="5">
-        <v>3</v>
-      </c>
-      <c r="C22" s="19">
-        <f t="shared" si="2"/>
-        <v>7.4921874999999997E-3</v>
-      </c>
-      <c r="D22" s="6">
-        <f t="shared" si="1"/>
-        <v>2.2476562499999998E-2</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="25">
-      <c r="A23" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="26">
+      <c r="B23" s="5">
         <v>3</v>
       </c>
       <c r="C23" s="19">
@@ -1878,314 +1911,332 @@
         <v>5</v>
       </c>
       <c r="F23" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="23">
+      <c r="A24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="21">
+        <v>3</v>
+      </c>
+      <c r="C24" s="19">
+        <f t="shared" si="2"/>
+        <v>7.4921874999999997E-3</v>
+      </c>
+      <c r="D24" s="6">
+        <f t="shared" si="1"/>
+        <v>2.2476562499999998E-2</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G23" s="36" t="s">
+      <c r="G24" s="31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="4" t="s">
+    <row r="25" spans="1:7" ht="17">
+      <c r="A25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B25" s="5">
         <v>2</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C25" s="19">
         <f>4.33/100</f>
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D25" s="6">
         <f t="shared" si="1"/>
         <v>8.6599999999999996E-2</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="92">
-      <c r="A25" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="26">
-        <v>1</v>
-      </c>
-      <c r="C25" s="38">
-        <v>9.99</v>
-      </c>
-      <c r="D25" s="6">
-        <f t="shared" ref="D25" si="4">B25*C25</f>
-        <v>9.99</v>
-      </c>
       <c r="E25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="100">
+      <c r="A26" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="21">
+        <v>1</v>
+      </c>
+      <c r="C26" s="33">
+        <v>9.99</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" ref="D26" si="4">B26*C26</f>
+        <v>9.99</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="G25" s="35" t="s">
+      <c r="G26" s="30" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-    </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-    </row>
-    <row r="28" spans="1:7" ht="30">
-      <c r="A28" s="4" t="s">
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+    </row>
+    <row r="29" spans="1:7" ht="34">
+      <c r="A29" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B28" s="5">
-        <v>1</v>
-      </c>
-      <c r="C28" s="6">
-        <v>10.86</v>
-      </c>
-      <c r="D28" s="6">
-        <f t="shared" ref="D28:D34" si="5">B28*C28</f>
-        <v>10.86</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
       </c>
       <c r="C29" s="6">
+        <v>10.86</v>
+      </c>
+      <c r="D29" s="6">
+        <f t="shared" ref="D29:D35" si="5">B29*C29</f>
+        <v>10.86</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="6">
+      <c r="F29" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" s="6">
+        <v>5</v>
+      </c>
+      <c r="D30" s="6">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="4" t="s">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" ht="17">
+      <c r="A31" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B31" s="5">
         <v>1</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C31" s="6">
         <v>4.5</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30">
-      <c r="A31" s="4" t="s">
+    <row r="32" spans="1:7" ht="34">
+      <c r="A32" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B32" s="5">
         <v>5</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C32" s="20">
         <f>16.3/125</f>
         <v>0.13040000000000002</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <f t="shared" si="5"/>
         <v>0.65200000000000014</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F32" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="45">
-      <c r="A32" s="4" t="s">
+    <row r="33" spans="1:6" ht="51">
+      <c r="A33" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B33" s="5">
         <v>3</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C33" s="20">
         <f>5.99/80</f>
         <v>7.4874999999999997E-2</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <f t="shared" si="5"/>
         <v>0.22462499999999999</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F33" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="26">
-      <c r="A33" s="4" t="s">
+    <row r="34" spans="1:6" ht="28">
+      <c r="A34" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B34" s="5">
         <v>10</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C34" s="6">
         <f>3.18/50</f>
         <v>6.3600000000000004E-2</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D34" s="6">
         <f t="shared" si="5"/>
         <v>0.63600000000000001</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F34" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="26">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:6" ht="28">
+      <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B35" s="5">
         <v>10</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C35" s="6">
         <f>5.49/100</f>
         <v>5.4900000000000004E-2</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <f t="shared" si="5"/>
         <v>0.54900000000000004</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-    </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="38"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="4" t="s">
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B38" s="5">
         <v>1</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C38" s="6">
         <v>5.2</v>
       </c>
-      <c r="D37" s="6">
-        <f>B37*C37</f>
+      <c r="D38" s="6">
+        <f>B38*C38</f>
         <v>5.2</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E38" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="13">
-        <f>SUM(D$3:D38)</f>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="13">
+        <f>SUM(D$4:D39)</f>
         <v>68.065113541666676</v>
       </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="14"/>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="E40" s="11"/>
       <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6">
       <c r="F41" s="14"/>
     </row>
-    <row r="42" spans="1:6" ht="16" customHeight="1">
-      <c r="A42" s="16"/>
+    <row r="42" spans="1:6">
       <c r="F42" s="14"/>
     </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="12"/>
+    <row r="43" spans="1:6" ht="16" customHeight="1">
+      <c r="A43" s="16"/>
       <c r="F43" s="14"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="17"/>
+      <c r="A44" s="12"/>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="12"/>
-      <c r="F45" s="14"/>
+      <c r="A45" s="17"/>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="12"/>
       <c r="F46" s="14"/>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="15"/>
+      <c r="A47" s="12"/>
       <c r="F47" s="14"/>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="12"/>
+      <c r="A48" s="15"/>
       <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:6">
@@ -2193,7 +2244,7 @@
       <c r="F49" s="14"/>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="15"/>
+      <c r="A50" s="12"/>
       <c r="F50" s="14"/>
     </row>
     <row r="51" spans="1:6">
@@ -2205,7 +2256,7 @@
       <c r="F52" s="14"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="12"/>
+      <c r="A53" s="15"/>
       <c r="F53" s="14"/>
     </row>
     <row r="54" spans="1:6">
@@ -2217,22 +2268,22 @@
       <c r="F55" s="14"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="9"/>
+      <c r="A56" s="12"/>
       <c r="F56" s="14"/>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="12"/>
+      <c r="A57" s="9"/>
       <c r="F57" s="14"/>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="12"/>
       <c r="F58" s="14"/>
     </row>
-    <row r="59" spans="1:6" ht="20" customHeight="1">
+    <row r="59" spans="1:6">
       <c r="A59" s="12"/>
       <c r="F59" s="14"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" ht="20" customHeight="1">
       <c r="A60" s="12"/>
       <c r="F60" s="14"/>
     </row>
@@ -2253,15 +2304,15 @@
       <c r="F64" s="14"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="18"/>
+      <c r="A65" s="12"/>
       <c r="F65" s="14"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="15"/>
+      <c r="A66" s="18"/>
       <c r="F66" s="14"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="12"/>
+      <c r="A67" s="15"/>
       <c r="F67" s="14"/>
     </row>
     <row r="68" spans="1:6">
@@ -2274,13 +2325,13 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="12"/>
+      <c r="F70" s="14"/>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="18"/>
-      <c r="F71" s="14"/>
+      <c r="A71" s="12"/>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="12"/>
+      <c r="A72" s="18"/>
       <c r="F72" s="14"/>
     </row>
     <row r="73" spans="1:6">
@@ -2308,11 +2359,12 @@
       <c r="F78" s="14"/>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="17"/>
+      <c r="A79" s="12"/>
       <c r="F79" s="14"/>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="17"/>
+      <c r="F80" s="14"/>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="17"/>
@@ -2374,19 +2426,23 @@
     <row r="100" spans="1:1">
       <c r="A100" s="17"/>
     </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="17"/>
+    </row>
   </sheetData>
-  <sortState ref="A26:F31">
-    <sortCondition descending="1" ref="C26:C31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A27:F32">
+    <sortCondition descending="1" ref="C27:C32"/>
   </sortState>
-  <mergeCells count="8">
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A2:F2"/>
+  <mergeCells count="9">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A28:F28"/>
     <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A27:F27"/>
     <mergeCell ref="A36:F36"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A35:F35"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>